<commit_message>
Added RRIDs to Donors file
</commit_message>
<xml_diff>
--- a/assets/metadata/latest/PancDB_Donors.xlsx
+++ b/assets/metadata/latest/PancDB_Donors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10817"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilanjanasamanta/Library/CloudStorage/Box-Box/HPAP-IBI/Pancdb-Metadata/current_v3.2.4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilanjanasamanta/Desktop/hpap-public/assets/metadata/latest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9098D3A6-0502-4A4D-8AB8-889481982309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9B8953-738E-904F-8236-8ABF8AA31C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32000" yWindow="-10860" windowWidth="21600" windowHeight="37900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="500" windowWidth="21600" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donors" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1686" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1708" uniqueCount="548">
   <si>
     <t xml:space="preserve">DonorID </t>
   </si>
@@ -1617,6 +1617,72 @@
   </si>
   <si>
     <t>Biracial</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701113</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701114</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701115</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701116</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701117</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701118</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701119</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701120</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701121</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RRID:SAMN50701123 </t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701124</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701125</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701126</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701127</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701128</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701129</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701130</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701131</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701132</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701133</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701134</t>
   </si>
 </sst>
 </file>
@@ -2261,10 +2327,10 @@
   <dimension ref="A1:CH193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B123" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B163" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F196" sqref="F196"/>
+      <selection pane="bottomRight" activeCell="D196" sqref="D196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -8925,6 +8991,9 @@
       <c r="A170" s="1" t="s">
         <v>500</v>
       </c>
+      <c r="B170" s="14" t="s">
+        <v>526</v>
+      </c>
       <c r="C170" s="39" t="s">
         <v>12</v>
       </c>
@@ -8954,6 +9023,9 @@
       <c r="A171" s="1" t="s">
         <v>501</v>
       </c>
+      <c r="B171" s="14" t="s">
+        <v>527</v>
+      </c>
       <c r="C171" s="39" t="s">
         <v>12</v>
       </c>
@@ -8983,6 +9055,9 @@
       <c r="A172" s="1" t="s">
         <v>502</v>
       </c>
+      <c r="B172" s="14" t="s">
+        <v>528</v>
+      </c>
       <c r="C172" s="39" t="s">
         <v>33</v>
       </c>
@@ -9012,6 +9087,9 @@
       <c r="A173" s="1" t="s">
         <v>503</v>
       </c>
+      <c r="B173" s="14" t="s">
+        <v>529</v>
+      </c>
       <c r="C173" s="39" t="s">
         <v>33</v>
       </c>
@@ -9041,6 +9119,9 @@
       <c r="A174" s="1" t="s">
         <v>504</v>
       </c>
+      <c r="B174" s="14" t="s">
+        <v>530</v>
+      </c>
       <c r="C174" s="39" t="s">
         <v>12</v>
       </c>
@@ -9070,6 +9151,9 @@
       <c r="A175" s="1" t="s">
         <v>505</v>
       </c>
+      <c r="B175" s="14" t="s">
+        <v>531</v>
+      </c>
       <c r="C175" s="39" t="s">
         <v>33</v>
       </c>
@@ -9099,6 +9183,9 @@
       <c r="A176" s="1" t="s">
         <v>506</v>
       </c>
+      <c r="B176" s="14" t="s">
+        <v>532</v>
+      </c>
       <c r="C176" s="39" t="s">
         <v>33</v>
       </c>
@@ -9128,6 +9215,9 @@
       <c r="A177" s="1" t="s">
         <v>507</v>
       </c>
+      <c r="B177" s="14" t="s">
+        <v>533</v>
+      </c>
       <c r="C177" s="39" t="s">
         <v>33</v>
       </c>
@@ -9157,6 +9247,9 @@
       <c r="A178" s="1" t="s">
         <v>508</v>
       </c>
+      <c r="B178" s="14" t="s">
+        <v>534</v>
+      </c>
       <c r="C178" s="39" t="s">
         <v>12</v>
       </c>
@@ -9186,6 +9279,9 @@
       <c r="A179" s="1" t="s">
         <v>509</v>
       </c>
+      <c r="B179" s="14" t="s">
+        <v>535</v>
+      </c>
       <c r="C179" s="51" t="s">
         <v>12</v>
       </c>
@@ -9215,6 +9311,9 @@
       <c r="A180" s="1" t="s">
         <v>510</v>
       </c>
+      <c r="B180" s="14" t="s">
+        <v>536</v>
+      </c>
       <c r="C180" s="39" t="s">
         <v>33</v>
       </c>
@@ -9244,6 +9343,9 @@
       <c r="A181" s="1" t="s">
         <v>511</v>
       </c>
+      <c r="B181" s="14" t="s">
+        <v>537</v>
+      </c>
       <c r="C181" s="39" t="s">
         <v>33</v>
       </c>
@@ -9273,6 +9375,9 @@
       <c r="A182" s="1" t="s">
         <v>513</v>
       </c>
+      <c r="B182" s="14" t="s">
+        <v>538</v>
+      </c>
       <c r="C182" s="39" t="s">
         <v>12</v>
       </c>
@@ -9299,6 +9404,9 @@
       <c r="A183" s="1" t="s">
         <v>514</v>
       </c>
+      <c r="B183" s="14" t="s">
+        <v>539</v>
+      </c>
       <c r="C183" s="39" t="s">
         <v>12</v>
       </c>
@@ -9325,6 +9433,9 @@
       <c r="A184" s="1" t="s">
         <v>515</v>
       </c>
+      <c r="B184" s="14" t="s">
+        <v>540</v>
+      </c>
       <c r="C184" s="39" t="s">
         <v>33</v>
       </c>
@@ -9351,6 +9462,9 @@
       <c r="A185" s="1" t="s">
         <v>516</v>
       </c>
+      <c r="B185" s="14" t="s">
+        <v>541</v>
+      </c>
       <c r="C185" s="39" t="s">
         <v>12</v>
       </c>
@@ -9377,6 +9491,9 @@
       <c r="A186" s="1" t="s">
         <v>517</v>
       </c>
+      <c r="B186" s="14" t="s">
+        <v>542</v>
+      </c>
       <c r="C186" s="39" t="s">
         <v>12</v>
       </c>
@@ -9403,6 +9520,9 @@
       <c r="A187" s="1" t="s">
         <v>518</v>
       </c>
+      <c r="B187" s="14" t="s">
+        <v>543</v>
+      </c>
       <c r="C187" s="39" t="s">
         <v>33</v>
       </c>
@@ -9429,6 +9549,9 @@
       <c r="A188" s="1" t="s">
         <v>519</v>
       </c>
+      <c r="B188" s="14" t="s">
+        <v>544</v>
+      </c>
       <c r="C188" s="39" t="s">
         <v>33</v>
       </c>
@@ -9452,6 +9575,9 @@
       <c r="A189" s="1" t="s">
         <v>520</v>
       </c>
+      <c r="B189" s="14" t="s">
+        <v>545</v>
+      </c>
       <c r="C189" s="39" t="s">
         <v>12</v>
       </c>
@@ -9475,6 +9601,9 @@
       <c r="A190" s="1" t="s">
         <v>521</v>
       </c>
+      <c r="B190" s="14" t="s">
+        <v>546</v>
+      </c>
       <c r="C190" s="39" t="s">
         <v>33</v>
       </c>
@@ -9498,6 +9627,9 @@
       <c r="A191" s="1" t="s">
         <v>522</v>
       </c>
+      <c r="B191" s="14" t="s">
+        <v>547</v>
+      </c>
       <c r="C191" s="39" t="s">
         <v>12</v>
       </c>
@@ -9529,7 +9661,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
-  <dataValidations count="15">
+  <dataValidations count="14">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"DonorID"</formula1>
     </dataValidation>
@@ -9551,7 +9683,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>"SampleSex"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12:E72 E77 E2:E10 E82:E164 E170:E194 E196:E1048576" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12:E72 E77 E2:E10 E82:E164 E170:E1048576" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>"American Indian or Alaska Native, Caucasian, Hispanic, Hispanic (MX), Asian, African american/Black, Biracial"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1" xr:uid="{00000000-0002-0000-0000-000009000000}">
@@ -9572,9 +9704,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11" xr:uid="{98871B29-57C8-4319-8DAA-5B4C3F03802F}">
       <formula1>"Caucasian, Hispanic, Hispanic (MX), Asian, African american/Black"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E195" xr:uid="{DF15A05D-29E1-234C-9366-591A9DDC3A1A}">
-      <formula1>"American Indian or Alaska Native, Caucasian, Hispanic, Hispanic (MX), Asian, African american/Black, Biracial"</formula1>
-    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added RRIDs to Donors file (#111)
</commit_message>
<xml_diff>
--- a/assets/metadata/latest/PancDB_Donors.xlsx
+++ b/assets/metadata/latest/PancDB_Donors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10817"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilanjanasamanta/Library/CloudStorage/Box-Box/HPAP-IBI/Pancdb-Metadata/current_v3.2.4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilanjanasamanta/Desktop/hpap-public/assets/metadata/latest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9098D3A6-0502-4A4D-8AB8-889481982309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9B8953-738E-904F-8236-8ABF8AA31C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32000" yWindow="-10860" windowWidth="21600" windowHeight="37900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="500" windowWidth="21600" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donors" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1686" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1708" uniqueCount="548">
   <si>
     <t xml:space="preserve">DonorID </t>
   </si>
@@ -1617,6 +1617,72 @@
   </si>
   <si>
     <t>Biracial</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701113</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701114</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701115</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701116</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701117</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701118</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701119</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701120</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701121</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RRID:SAMN50701123 </t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701124</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701125</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701126</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701127</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701128</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701129</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701130</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701131</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701132</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701133</t>
+  </si>
+  <si>
+    <t>RRID:SAMN50701134</t>
   </si>
 </sst>
 </file>
@@ -2261,10 +2327,10 @@
   <dimension ref="A1:CH193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B123" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B163" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F196" sqref="F196"/>
+      <selection pane="bottomRight" activeCell="D196" sqref="D196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -8925,6 +8991,9 @@
       <c r="A170" s="1" t="s">
         <v>500</v>
       </c>
+      <c r="B170" s="14" t="s">
+        <v>526</v>
+      </c>
       <c r="C170" s="39" t="s">
         <v>12</v>
       </c>
@@ -8954,6 +9023,9 @@
       <c r="A171" s="1" t="s">
         <v>501</v>
       </c>
+      <c r="B171" s="14" t="s">
+        <v>527</v>
+      </c>
       <c r="C171" s="39" t="s">
         <v>12</v>
       </c>
@@ -8983,6 +9055,9 @@
       <c r="A172" s="1" t="s">
         <v>502</v>
       </c>
+      <c r="B172" s="14" t="s">
+        <v>528</v>
+      </c>
       <c r="C172" s="39" t="s">
         <v>33</v>
       </c>
@@ -9012,6 +9087,9 @@
       <c r="A173" s="1" t="s">
         <v>503</v>
       </c>
+      <c r="B173" s="14" t="s">
+        <v>529</v>
+      </c>
       <c r="C173" s="39" t="s">
         <v>33</v>
       </c>
@@ -9041,6 +9119,9 @@
       <c r="A174" s="1" t="s">
         <v>504</v>
       </c>
+      <c r="B174" s="14" t="s">
+        <v>530</v>
+      </c>
       <c r="C174" s="39" t="s">
         <v>12</v>
       </c>
@@ -9070,6 +9151,9 @@
       <c r="A175" s="1" t="s">
         <v>505</v>
       </c>
+      <c r="B175" s="14" t="s">
+        <v>531</v>
+      </c>
       <c r="C175" s="39" t="s">
         <v>33</v>
       </c>
@@ -9099,6 +9183,9 @@
       <c r="A176" s="1" t="s">
         <v>506</v>
       </c>
+      <c r="B176" s="14" t="s">
+        <v>532</v>
+      </c>
       <c r="C176" s="39" t="s">
         <v>33</v>
       </c>
@@ -9128,6 +9215,9 @@
       <c r="A177" s="1" t="s">
         <v>507</v>
       </c>
+      <c r="B177" s="14" t="s">
+        <v>533</v>
+      </c>
       <c r="C177" s="39" t="s">
         <v>33</v>
       </c>
@@ -9157,6 +9247,9 @@
       <c r="A178" s="1" t="s">
         <v>508</v>
       </c>
+      <c r="B178" s="14" t="s">
+        <v>534</v>
+      </c>
       <c r="C178" s="39" t="s">
         <v>12</v>
       </c>
@@ -9186,6 +9279,9 @@
       <c r="A179" s="1" t="s">
         <v>509</v>
       </c>
+      <c r="B179" s="14" t="s">
+        <v>535</v>
+      </c>
       <c r="C179" s="51" t="s">
         <v>12</v>
       </c>
@@ -9215,6 +9311,9 @@
       <c r="A180" s="1" t="s">
         <v>510</v>
       </c>
+      <c r="B180" s="14" t="s">
+        <v>536</v>
+      </c>
       <c r="C180" s="39" t="s">
         <v>33</v>
       </c>
@@ -9244,6 +9343,9 @@
       <c r="A181" s="1" t="s">
         <v>511</v>
       </c>
+      <c r="B181" s="14" t="s">
+        <v>537</v>
+      </c>
       <c r="C181" s="39" t="s">
         <v>33</v>
       </c>
@@ -9273,6 +9375,9 @@
       <c r="A182" s="1" t="s">
         <v>513</v>
       </c>
+      <c r="B182" s="14" t="s">
+        <v>538</v>
+      </c>
       <c r="C182" s="39" t="s">
         <v>12</v>
       </c>
@@ -9299,6 +9404,9 @@
       <c r="A183" s="1" t="s">
         <v>514</v>
       </c>
+      <c r="B183" s="14" t="s">
+        <v>539</v>
+      </c>
       <c r="C183" s="39" t="s">
         <v>12</v>
       </c>
@@ -9325,6 +9433,9 @@
       <c r="A184" s="1" t="s">
         <v>515</v>
       </c>
+      <c r="B184" s="14" t="s">
+        <v>540</v>
+      </c>
       <c r="C184" s="39" t="s">
         <v>33</v>
       </c>
@@ -9351,6 +9462,9 @@
       <c r="A185" s="1" t="s">
         <v>516</v>
       </c>
+      <c r="B185" s="14" t="s">
+        <v>541</v>
+      </c>
       <c r="C185" s="39" t="s">
         <v>12</v>
       </c>
@@ -9377,6 +9491,9 @@
       <c r="A186" s="1" t="s">
         <v>517</v>
       </c>
+      <c r="B186" s="14" t="s">
+        <v>542</v>
+      </c>
       <c r="C186" s="39" t="s">
         <v>12</v>
       </c>
@@ -9403,6 +9520,9 @@
       <c r="A187" s="1" t="s">
         <v>518</v>
       </c>
+      <c r="B187" s="14" t="s">
+        <v>543</v>
+      </c>
       <c r="C187" s="39" t="s">
         <v>33</v>
       </c>
@@ -9429,6 +9549,9 @@
       <c r="A188" s="1" t="s">
         <v>519</v>
       </c>
+      <c r="B188" s="14" t="s">
+        <v>544</v>
+      </c>
       <c r="C188" s="39" t="s">
         <v>33</v>
       </c>
@@ -9452,6 +9575,9 @@
       <c r="A189" s="1" t="s">
         <v>520</v>
       </c>
+      <c r="B189" s="14" t="s">
+        <v>545</v>
+      </c>
       <c r="C189" s="39" t="s">
         <v>12</v>
       </c>
@@ -9475,6 +9601,9 @@
       <c r="A190" s="1" t="s">
         <v>521</v>
       </c>
+      <c r="B190" s="14" t="s">
+        <v>546</v>
+      </c>
       <c r="C190" s="39" t="s">
         <v>33</v>
       </c>
@@ -9498,6 +9627,9 @@
       <c r="A191" s="1" t="s">
         <v>522</v>
       </c>
+      <c r="B191" s="14" t="s">
+        <v>547</v>
+      </c>
       <c r="C191" s="39" t="s">
         <v>12</v>
       </c>
@@ -9529,7 +9661,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
-  <dataValidations count="15">
+  <dataValidations count="14">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"DonorID"</formula1>
     </dataValidation>
@@ -9551,7 +9683,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>"SampleSex"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12:E72 E77 E2:E10 E82:E164 E170:E194 E196:E1048576" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12:E72 E77 E2:E10 E82:E164 E170:E1048576" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>"American Indian or Alaska Native, Caucasian, Hispanic, Hispanic (MX), Asian, African american/Black, Biracial"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1" xr:uid="{00000000-0002-0000-0000-000009000000}">
@@ -9572,9 +9704,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11" xr:uid="{98871B29-57C8-4319-8DAA-5B4C3F03802F}">
       <formula1>"Caucasian, Hispanic, Hispanic (MX), Asian, African american/Black"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E195" xr:uid="{DF15A05D-29E1-234C-9366-591A9DDC3A1A}">
-      <formula1>"American Indian or Alaska Native, Caucasian, Hispanic, Hispanic (MX), Asian, African american/Black, Biracial"</formula1>
-    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
releasing metadata V4.0.1 (#120)
Co-authored-by: Nilanjana Samanta <nilanjanasamanta@faryabi21.pmacs.upenn.edu>
Co-authored-by: yimsheng <jamiesheng0306@gmail.com>
</commit_message>
<xml_diff>
--- a/assets/metadata/latest/PancDB_Donors.xlsx
+++ b/assets/metadata/latest/PancDB_Donors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilanjanasamanta/Desktop/hpap-public/assets/metadata/latest/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilanjanasamanta/Library/CloudStorage/Box-Box/HPAP-IBI/Pancdb-Metadata/current_v4.1.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9B8953-738E-904F-8236-8ABF8AA31C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3235D056-7D0E-374A-8B8B-5C98DDB334A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="500" windowWidth="21600" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32000" yWindow="-10860" windowWidth="21600" windowHeight="37900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donors" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1708" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="527">
   <si>
     <t xml:space="preserve">DonorID </t>
   </si>
@@ -1619,70 +1619,7 @@
     <t>Biracial</t>
   </si>
   <si>
-    <t>RRID:SAMN50701113</t>
-  </si>
-  <si>
-    <t>RRID:SAMN50701114</t>
-  </si>
-  <si>
-    <t>RRID:SAMN50701115</t>
-  </si>
-  <si>
-    <t>RRID:SAMN50701116</t>
-  </si>
-  <si>
-    <t>RRID:SAMN50701117</t>
-  </si>
-  <si>
-    <t>RRID:SAMN50701118</t>
-  </si>
-  <si>
-    <t>RRID:SAMN50701119</t>
-  </si>
-  <si>
-    <t>RRID:SAMN50701120</t>
-  </si>
-  <si>
-    <t>RRID:SAMN50701121</t>
-  </si>
-  <si>
-    <t>RRID:SAMN50701122</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RRID:SAMN50701123 </t>
-  </si>
-  <si>
-    <t>RRID:SAMN50701124</t>
-  </si>
-  <si>
-    <t>RRID:SAMN50701125</t>
-  </si>
-  <si>
-    <t>RRID:SAMN50701126</t>
-  </si>
-  <si>
-    <t>RRID:SAMN50701127</t>
-  </si>
-  <si>
-    <t>RRID:SAMN50701128</t>
-  </si>
-  <si>
-    <t>RRID:SAMN50701129</t>
-  </si>
-  <si>
-    <t>RRID:SAMN50701130</t>
-  </si>
-  <si>
-    <t>RRID:SAMN50701131</t>
-  </si>
-  <si>
-    <t>RRID:SAMN50701132</t>
-  </si>
-  <si>
-    <t>RRID:SAMN50701133</t>
-  </si>
-  <si>
-    <t>RRID:SAMN50701134</t>
+    <t>HPAP-196</t>
   </si>
 </sst>
 </file>
@@ -2324,13 +2261,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CH193"/>
+  <dimension ref="A1:CH194"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B163" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B108" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D196" sqref="D196"/>
+      <selection pane="bottomRight" activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -7359,7 +7296,7 @@
       <c r="A119" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="B119" s="39" t="s">
+      <c r="B119" s="14" t="s">
         <v>413</v>
       </c>
       <c r="C119" s="39" t="s">
@@ -8991,9 +8928,6 @@
       <c r="A170" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="B170" s="14" t="s">
-        <v>526</v>
-      </c>
       <c r="C170" s="39" t="s">
         <v>12</v>
       </c>
@@ -9023,9 +8957,6 @@
       <c r="A171" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="B171" s="14" t="s">
-        <v>527</v>
-      </c>
       <c r="C171" s="39" t="s">
         <v>12</v>
       </c>
@@ -9055,9 +8986,6 @@
       <c r="A172" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="B172" s="14" t="s">
-        <v>528</v>
-      </c>
       <c r="C172" s="39" t="s">
         <v>33</v>
       </c>
@@ -9087,9 +9015,6 @@
       <c r="A173" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="B173" s="14" t="s">
-        <v>529</v>
-      </c>
       <c r="C173" s="39" t="s">
         <v>33</v>
       </c>
@@ -9119,9 +9044,6 @@
       <c r="A174" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="B174" s="14" t="s">
-        <v>530</v>
-      </c>
       <c r="C174" s="39" t="s">
         <v>12</v>
       </c>
@@ -9151,9 +9073,6 @@
       <c r="A175" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="B175" s="14" t="s">
-        <v>531</v>
-      </c>
       <c r="C175" s="39" t="s">
         <v>33</v>
       </c>
@@ -9183,9 +9102,6 @@
       <c r="A176" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="B176" s="14" t="s">
-        <v>532</v>
-      </c>
       <c r="C176" s="39" t="s">
         <v>33</v>
       </c>
@@ -9215,9 +9131,6 @@
       <c r="A177" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="B177" s="14" t="s">
-        <v>533</v>
-      </c>
       <c r="C177" s="39" t="s">
         <v>33</v>
       </c>
@@ -9247,9 +9160,6 @@
       <c r="A178" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="B178" s="14" t="s">
-        <v>534</v>
-      </c>
       <c r="C178" s="39" t="s">
         <v>12</v>
       </c>
@@ -9279,9 +9189,6 @@
       <c r="A179" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="B179" s="14" t="s">
-        <v>535</v>
-      </c>
       <c r="C179" s="51" t="s">
         <v>12</v>
       </c>
@@ -9311,9 +9218,6 @@
       <c r="A180" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="B180" s="14" t="s">
-        <v>536</v>
-      </c>
       <c r="C180" s="39" t="s">
         <v>33</v>
       </c>
@@ -9343,9 +9247,6 @@
       <c r="A181" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="B181" s="14" t="s">
-        <v>537</v>
-      </c>
       <c r="C181" s="39" t="s">
         <v>33</v>
       </c>
@@ -9375,9 +9276,6 @@
       <c r="A182" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="B182" s="14" t="s">
-        <v>538</v>
-      </c>
       <c r="C182" s="39" t="s">
         <v>12</v>
       </c>
@@ -9397,6 +9295,9 @@
         <v>24</v>
       </c>
       <c r="I182" s="17" t="s">
+        <v>470</v>
+      </c>
+      <c r="J182" s="17" t="s">
         <v>470</v>
       </c>
     </row>
@@ -9404,9 +9305,6 @@
       <c r="A183" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="B183" s="14" t="s">
-        <v>539</v>
-      </c>
       <c r="C183" s="39" t="s">
         <v>12</v>
       </c>
@@ -9426,6 +9324,9 @@
         <v>17</v>
       </c>
       <c r="I183" s="17" t="s">
+        <v>470</v>
+      </c>
+      <c r="J183" s="17" t="s">
         <v>470</v>
       </c>
     </row>
@@ -9433,9 +9334,6 @@
       <c r="A184" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="B184" s="14" t="s">
-        <v>540</v>
-      </c>
       <c r="C184" s="39" t="s">
         <v>33</v>
       </c>
@@ -9455,6 +9353,9 @@
         <v>24</v>
       </c>
       <c r="I184" s="17" t="s">
+        <v>470</v>
+      </c>
+      <c r="J184" s="17" t="s">
         <v>470</v>
       </c>
     </row>
@@ -9462,9 +9363,6 @@
       <c r="A185" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="B185" s="14" t="s">
-        <v>541</v>
-      </c>
       <c r="C185" s="39" t="s">
         <v>12</v>
       </c>
@@ -9484,6 +9382,9 @@
         <v>17</v>
       </c>
       <c r="I185" s="17" t="s">
+        <v>470</v>
+      </c>
+      <c r="J185" s="17" t="s">
         <v>470</v>
       </c>
     </row>
@@ -9491,9 +9392,6 @@
       <c r="A186" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="B186" s="14" t="s">
-        <v>542</v>
-      </c>
       <c r="C186" s="39" t="s">
         <v>12</v>
       </c>
@@ -9513,6 +9411,9 @@
         <v>24</v>
       </c>
       <c r="I186" s="17" t="s">
+        <v>470</v>
+      </c>
+      <c r="J186" s="17" t="s">
         <v>470</v>
       </c>
     </row>
@@ -9520,9 +9421,6 @@
       <c r="A187" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="B187" s="14" t="s">
-        <v>543</v>
-      </c>
       <c r="C187" s="39" t="s">
         <v>33</v>
       </c>
@@ -9542,6 +9440,9 @@
         <v>17</v>
       </c>
       <c r="I187" s="17" t="s">
+        <v>470</v>
+      </c>
+      <c r="J187" s="17" t="s">
         <v>470</v>
       </c>
     </row>
@@ -9549,9 +9450,6 @@
       <c r="A188" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="B188" s="14" t="s">
-        <v>544</v>
-      </c>
       <c r="C188" s="39" t="s">
         <v>33</v>
       </c>
@@ -9569,15 +9467,18 @@
       </c>
       <c r="H188" s="39" t="s">
         <v>24</v>
+      </c>
+      <c r="I188" s="17" t="s">
+        <v>470</v>
+      </c>
+      <c r="J188" s="17" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="189" spans="1:10">
       <c r="A189" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="B189" s="14" t="s">
-        <v>545</v>
-      </c>
       <c r="C189" s="39" t="s">
         <v>12</v>
       </c>
@@ -9595,15 +9496,18 @@
       </c>
       <c r="H189" s="39" t="s">
         <v>17</v>
+      </c>
+      <c r="I189" s="17" t="s">
+        <v>470</v>
+      </c>
+      <c r="J189" s="17" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="190" spans="1:10">
       <c r="A190" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="B190" s="14" t="s">
-        <v>546</v>
-      </c>
       <c r="C190" s="39" t="s">
         <v>33</v>
       </c>
@@ -9621,15 +9525,18 @@
       </c>
       <c r="H190" s="39" t="s">
         <v>17</v>
+      </c>
+      <c r="I190" s="17" t="s">
+        <v>470</v>
+      </c>
+      <c r="J190" s="17" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="191" spans="1:10">
       <c r="A191" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="B191" s="14" t="s">
-        <v>547</v>
-      </c>
       <c r="C191" s="39" t="s">
         <v>12</v>
       </c>
@@ -9647,16 +9554,75 @@
       </c>
       <c r="H191" s="39" t="s">
         <v>17</v>
+      </c>
+      <c r="I191" s="17" t="s">
+        <v>470</v>
+      </c>
+      <c r="J191" s="17" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="192" spans="1:10">
       <c r="A192" s="1" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="193" spans="1:1">
+      <c r="C192" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="D192" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="E192" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F192" s="39" t="s">
+        <v>231</v>
+      </c>
+      <c r="G192" s="56" t="s">
+        <v>289</v>
+      </c>
+      <c r="H192" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="I192" s="17" t="s">
+        <v>470</v>
+      </c>
+      <c r="J192" s="17" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10">
       <c r="A193" s="1" t="s">
         <v>524</v>
+      </c>
+      <c r="C193" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D193" s="39" t="s">
+        <v>499</v>
+      </c>
+      <c r="E193" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F193" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="G193" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H193" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="I193" s="17" t="s">
+        <v>470</v>
+      </c>
+      <c r="J193" s="17" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10">
+      <c r="A194" s="1" t="s">
+        <v>526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>